<commit_message>
forgot to print some output but its alright now
</commit_message>
<xml_diff>
--- a/iets.xlsx
+++ b/iets.xlsx
@@ -397,22 +397,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.1855516988434487</v>
+        <v>0.03742607606442153</v>
       </c>
       <c r="C2">
-        <v>0.1489126539843185</v>
+        <v>0.01735433991663465</v>
       </c>
       <c r="D2">
-        <v>0.006270397224164095</v>
+        <v>0.03506375804688142</v>
       </c>
       <c r="E2">
-        <v>0.006948461444066759</v>
+        <v>0.008118037228071846</v>
       </c>
       <c r="F2">
-        <v>0.05346985975038727</v>
+        <v>0.03682596592847593</v>
       </c>
       <c r="G2">
-        <v>0.02489367035155918</v>
+        <v>0.0200845498731792</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -420,22 +420,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.05005339988782809</v>
+        <v>0.02806055989938596</v>
       </c>
       <c r="C3">
-        <v>0.04876983274944631</v>
+        <v>0.0287711510192422</v>
       </c>
       <c r="D3">
-        <v>0.02785413421582113</v>
+        <v>0.04918539443472066</v>
       </c>
       <c r="E3">
-        <v>0.0280912878342478</v>
+        <v>0.04911947615978158</v>
       </c>
       <c r="F3">
-        <v>0.03785376544892448</v>
+        <v>0.01928526081147312</v>
       </c>
       <c r="G3">
-        <v>0.03835489619499917</v>
+        <v>0.01986233663867399</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -443,22 +443,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.05140012547116234</v>
+        <v>0.03646409467464339</v>
       </c>
       <c r="C4">
-        <v>0.08543237227868804</v>
+        <v>0.03580779814367356</v>
       </c>
       <c r="D4">
-        <v>0.0001880400280942968</v>
+        <v>0.02011035498457307</v>
       </c>
       <c r="E4">
-        <v>0.0004398614728402359</v>
+        <v>0.02754968594147661</v>
       </c>
       <c r="F4">
-        <v>0.01112926963087568</v>
+        <v>0.01064380226166979</v>
       </c>
       <c r="G4">
-        <v>0.02473630162422272</v>
+        <v>0.01048723923400685</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -466,22 +466,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.02946246989721811</v>
+        <v>0.02118225111743641</v>
       </c>
       <c r="C5">
-        <v>0.03301700888534305</v>
+        <v>0.02103491568459112</v>
       </c>
       <c r="D5">
-        <v>7.646180562119085e-05</v>
+        <v>0.01033833192424172</v>
       </c>
       <c r="E5">
-        <v>0.0001610022310280388</v>
+        <v>0.01145276069530116</v>
       </c>
       <c r="F5">
-        <v>0.009475356095681065</v>
+        <v>0.004932906579649861</v>
       </c>
       <c r="G5">
-        <v>0.01065893286810568</v>
+        <v>0.00466256026706771</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -489,22 +489,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.07179879263363315</v>
+        <v>0.1452262427004578</v>
       </c>
       <c r="C6">
-        <v>0.003156804136280866</v>
+        <v>0.03881545611889942</v>
       </c>
       <c r="D6">
-        <v>0.1273827383895082</v>
+        <v>0.0815887606899436</v>
       </c>
       <c r="E6">
-        <v>0.05963044068275524</v>
+        <v>0.02910867774809549</v>
       </c>
       <c r="F6">
-        <v>0.0796243856874206</v>
+        <v>0.1165753023852861</v>
       </c>
       <c r="G6">
-        <v>0.02422513256487388</v>
+        <v>0.04179805946082008</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -512,22 +512,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.02142302774952111</v>
+        <v>0.0399857475402855</v>
       </c>
       <c r="C7">
-        <v>0.001630229422204268</v>
+        <v>0.02953529607767487</v>
       </c>
       <c r="D7">
-        <v>0.02451524061264081</v>
+        <v>0.01651853452041685</v>
       </c>
       <c r="E7">
-        <v>0.02877174041297381</v>
+        <v>0.01555199674721331</v>
       </c>
       <c r="F7">
-        <v>0.01734124927898775</v>
+        <v>0.02569016821914447</v>
       </c>
       <c r="G7">
-        <v>0.01415202003449306</v>
+        <v>0.01949593085650963</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -535,22 +535,22 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.9292414617410149</v>
+        <v>0.8637590537089674</v>
       </c>
       <c r="C8">
-        <v>0.9363938198878868</v>
+        <v>0.8861858005738782</v>
       </c>
       <c r="D8">
-        <v>0.8992235324571751</v>
+        <v>0.9314824565938706</v>
       </c>
       <c r="E8">
-        <v>0.9175909683253339</v>
+        <v>0.9385707458446433</v>
       </c>
       <c r="F8">
-        <v>0.9291669050879098</v>
+        <v>0.8905505363486729</v>
       </c>
       <c r="G8">
-        <v>0.9317507432906799</v>
+        <v>0.9051044498576281</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -558,22 +558,22 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.02159498833767121</v>
+        <v>0.04121757406691675</v>
       </c>
       <c r="C9">
-        <v>0.01674160464637454</v>
+        <v>0.04200305340334829</v>
       </c>
       <c r="D9">
-        <v>0.01786131870752281</v>
+        <v>0.01340434543259565</v>
       </c>
       <c r="E9">
-        <v>0.0197545261398785</v>
+        <v>0.01338077594820928</v>
       </c>
       <c r="F9">
-        <v>0.01511081867555608</v>
+        <v>0.02398291086272598</v>
       </c>
       <c r="G9">
-        <v>0.01570095700485885</v>
+        <v>0.02193740716661464</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -581,13 +581,13 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>0.1084270318514724</v>
+        <v>0.1602595465005063</v>
       </c>
       <c r="E10">
-        <v>0.08905135805330211</v>
+        <v>0.08749139758189517</v>
       </c>
       <c r="G10">
-        <v>0.09551307605564907</v>
+        <v>0.1196837274874851</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -595,13 +595,13 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>0.02952000435489707</v>
+        <v>0.04229280253821115</v>
       </c>
       <c r="E11">
-        <v>0.02155356129794989</v>
+        <v>0.02344653717128905</v>
       </c>
       <c r="G11">
-        <v>0.02629988233948873</v>
+        <v>0.02840974511261153</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -609,22 +609,22 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>5.909014947315913</v>
+        <v>4.291113069285608</v>
       </c>
       <c r="C12">
-        <v>5.903662796568089</v>
+        <v>4.329020436629127</v>
       </c>
       <c r="D12">
-        <v>4.974933914211391</v>
+        <v>3.872445733506573</v>
       </c>
       <c r="E12">
-        <v>5.032937063566784</v>
+        <v>3.891870898365699</v>
       </c>
       <c r="F12">
-        <v>6.421567543680288</v>
+        <v>6.698973456559248</v>
       </c>
       <c r="G12">
-        <v>6.558441159847681</v>
+        <v>7.095796123900807</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -632,22 +632,22 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.7526885217309252</v>
+        <v>0.4186904290563454</v>
       </c>
       <c r="C13">
-        <v>0.7356570228405572</v>
+        <v>0.4159186518916121</v>
       </c>
       <c r="D13">
-        <v>0.5200325066832139</v>
+        <v>0.332751578697806</v>
       </c>
       <c r="E13">
-        <v>0.5328960962892375</v>
+        <v>0.3363378721560813</v>
       </c>
       <c r="F13">
-        <v>0.7622524723415345</v>
+        <v>0.7775384444035005</v>
       </c>
       <c r="G13">
-        <v>0.7650290648829928</v>
+        <v>0.8625573269246137</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -655,22 +655,22 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-6098.763675972762</v>
+        <v>-4833.862741016288</v>
       </c>
       <c r="C14">
-        <v>-6092.816229124846</v>
+        <v>-4818.973508420826</v>
       </c>
       <c r="D14">
-        <v>-4935.803406424151</v>
+        <v>-6441.222436456836</v>
       </c>
       <c r="E14">
-        <v>-4927.455765907544</v>
+        <v>-6433.000686815352</v>
       </c>
       <c r="F14">
-        <v>-5722.011619031751</v>
+        <v>-3961.195665966567</v>
       </c>
       <c r="G14">
-        <v>-5710.693636478363</v>
+        <v>-3949.595743188088</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -678,22 +678,22 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>12205.52735194552</v>
+        <v>9675.725482032576</v>
       </c>
       <c r="C15">
-        <v>12195.63245824969</v>
+        <v>9647.947016841652</v>
       </c>
       <c r="D15">
-        <v>9879.606812848302</v>
+        <v>12890.44487291367</v>
       </c>
       <c r="E15">
-        <v>9864.911531815087</v>
+        <v>12876.0013736307</v>
       </c>
       <c r="F15">
-        <v>11452.0232380635</v>
+        <v>7930.391331933134</v>
       </c>
       <c r="G15">
-        <v>11431.38727295673</v>
+        <v>7909.191486376176</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -701,22 +701,22 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>12228.82353598895</v>
+        <v>9699.021666076002</v>
       </c>
       <c r="C16">
-        <v>12224.75268830397</v>
+        <v>9677.067246895933</v>
       </c>
       <c r="D16">
-        <v>9902.902996891728</v>
+        <v>12913.7410569571</v>
       </c>
       <c r="E16">
-        <v>9894.031761869368</v>
+        <v>12905.12160368499</v>
       </c>
       <c r="F16">
-        <v>11475.31942210693</v>
+        <v>7953.68751597656</v>
       </c>
       <c r="G16">
-        <v>11460.50750301101</v>
+        <v>7938.311716430458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>